<commit_message>
GPLIM-1307:  Updates to Parser with updates to Test Coverage
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/quant_upload_good.xlsx
+++ b/mercury/src/test/resources/testdata/quant_upload_good.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t>Location</t>
   </si>
@@ -220,6 +220,51 @@
   </si>
   <si>
     <t>H8</t>
+  </si>
+  <si>
+    <t>SGMTEST2402938482</t>
+  </si>
+  <si>
+    <t>SGMTEST2208428758</t>
+  </si>
+  <si>
+    <t>SGMTEST3559709487</t>
+  </si>
+  <si>
+    <t>SGMTEST3938342818</t>
+  </si>
+  <si>
+    <t>SGMTEST3585528276</t>
+  </si>
+  <si>
+    <t>SGMTEST3132943337</t>
+  </si>
+  <si>
+    <t>SGMTEST8815228500</t>
+  </si>
+  <si>
+    <t>SGMTEST5936483766</t>
+  </si>
+  <si>
+    <t>SGMTEST4621329996</t>
+  </si>
+  <si>
+    <t>SGMTEST9085949196</t>
+  </si>
+  <si>
+    <t>SGMTEST4069756425</t>
+  </si>
+  <si>
+    <t>SGMTEST3850486410</t>
+  </si>
+  <si>
+    <t>SGMTEST5761812024</t>
+  </si>
+  <si>
+    <t>SGMTEST4047896363</t>
+  </si>
+  <si>
+    <t>SGMTEST5142352881</t>
   </si>
 </sst>
 </file>
@@ -672,12 +717,12 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -695,8 +740,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>2402938482</v>
+      <c r="B2" t="s">
+        <v>67</v>
       </c>
       <c r="C2" s="1">
         <v>32.42</v>
@@ -706,8 +751,8 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
-        <v>2208428758</v>
+      <c r="B3" t="s">
+        <v>68</v>
       </c>
       <c r="C3" s="1">
         <v>54.22</v>
@@ -717,8 +762,8 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>3559709487</v>
+      <c r="B4" t="s">
+        <v>69</v>
       </c>
       <c r="C4" s="1">
         <v>17.760000000000002</v>
@@ -728,8 +773,8 @@
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
-        <v>3938342818</v>
+      <c r="B5" t="s">
+        <v>70</v>
       </c>
       <c r="C5" s="1">
         <v>16.22</v>
@@ -739,8 +784,8 @@
       <c r="A6" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>3585528276</v>
+      <c r="B6" t="s">
+        <v>71</v>
       </c>
       <c r="C6" s="1">
         <v>62.74</v>
@@ -750,8 +795,8 @@
       <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>3132943337</v>
+      <c r="B7" t="s">
+        <v>72</v>
       </c>
       <c r="C7" s="1">
         <v>99.11</v>
@@ -761,8 +806,8 @@
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>8815228500</v>
+      <c r="B8" t="s">
+        <v>73</v>
       </c>
       <c r="C8" s="1">
         <v>42.09</v>
@@ -772,8 +817,8 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>5936483766</v>
+      <c r="B9" t="s">
+        <v>74</v>
       </c>
       <c r="C9" s="1">
         <v>28.04</v>
@@ -783,8 +828,8 @@
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>4621329996</v>
+      <c r="B10" t="s">
+        <v>75</v>
       </c>
       <c r="C10" s="1">
         <v>95.05</v>
@@ -794,8 +839,8 @@
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11">
-        <v>9085949196</v>
+      <c r="B11" t="s">
+        <v>76</v>
       </c>
       <c r="C11" s="1">
         <v>41.21</v>
@@ -805,8 +850,8 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12">
-        <v>4069756425</v>
+      <c r="B12" t="s">
+        <v>77</v>
       </c>
       <c r="C12" s="1">
         <v>71.66</v>
@@ -816,8 +861,8 @@
       <c r="A13" t="s">
         <v>32</v>
       </c>
-      <c r="B13">
-        <v>3850486410</v>
+      <c r="B13" t="s">
+        <v>78</v>
       </c>
       <c r="C13" s="1">
         <v>59.02</v>
@@ -827,8 +872,8 @@
       <c r="A14" t="s">
         <v>39</v>
       </c>
-      <c r="B14">
-        <v>5761812024</v>
+      <c r="B14" t="s">
+        <v>79</v>
       </c>
       <c r="C14" s="1">
         <v>50.44</v>
@@ -838,8 +883,8 @@
       <c r="A15" t="s">
         <v>46</v>
       </c>
-      <c r="B15">
-        <v>4047896363</v>
+      <c r="B15" t="s">
+        <v>80</v>
       </c>
       <c r="C15" s="1">
         <v>33.950000000000003</v>
@@ -849,8 +894,8 @@
       <c r="A16" t="s">
         <v>53</v>
       </c>
-      <c r="B16">
-        <v>5142352881</v>
+      <c r="B16" t="s">
+        <v>81</v>
       </c>
       <c r="C16" s="1">
         <v>38.44</v>

</xml_diff>